<commit_message>
Iterator, Object, Automation Overview, Framework Overview
</commit_message>
<xml_diff>
--- a/src/main/resources/AutoTestData.xlsx
+++ b/src/main/resources/AutoTestData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\eclipse-workspace\com.geico.qa\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66630D6B-E405-40E2-B6A7-76E4E3D9C78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBF4DDE-7917-4294-824E-A78EF4F1310B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A5E35C8D-228A-4A70-BF93-D37071E14EB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A5E35C8D-228A-4A70-BF93-D37071E14EB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Maps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t>Test No</t>
   </si>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F161BE-8528-428C-99DD-14F54FA3841E}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,12 +747,224 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356677E8-C5F7-45D7-8ED1-98D8ADDE0F88}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{BC1173F0-5FC5-42E2-ADE9-515ACDCF2E03}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{FEF6D58C-6D9D-4B1A-A5E7-1A590B5936A9}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{A82A19F1-80A8-40BC-AA5C-46ECF68FC513}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{430841FA-23F0-447D-8A6D-D53B133A89D2}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{A52327F0-48A5-46C5-AED7-E5741235AF1B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Map DataProvider, Enum with String value
</commit_message>
<xml_diff>
--- a/src/main/resources/AutoTestData.xlsx
+++ b/src/main/resources/AutoTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\eclipse-workspace\com.geico.qa\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBF4DDE-7917-4294-824E-A78EF4F1310B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD6D90B-9393-4F01-A353-19FDA3E2CDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A5E35C8D-228A-4A70-BF93-D37071E14EB7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
   <si>
     <t>Test No</t>
   </si>
@@ -144,6 +144,30 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>hjhu</t>
+  </si>
+  <si>
+    <t>lkl</t>
+  </si>
+  <si>
+    <t>b vb</t>
+  </si>
+  <si>
+    <t>bh</t>
+  </si>
+  <si>
+    <t>kldjk</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -203,11 +227,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -747,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356677E8-C5F7-45D7-8ED1-98D8ADDE0F88}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,194 +795,241 @@
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="6" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>